<commit_message>
modified home,added seperate pages,styled
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Exam-Seat-Arrangement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68D388C-F63E-47B8-9D17-CD3F84731869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C3694A-12D3-43D5-9884-062E148EA7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>